<commit_message>
3rd Commit of konakart.com parallel with Waits and WebTable handling class
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="7935" activeTab="6"/>
+    <workbookView windowWidth="20385" windowHeight="8355" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
   <si>
     <t>TestData</t>
   </si>
@@ -143,13 +143,16 @@
     <t>com.konakart.KonakartParallelTesting.testscripts.HeroImageFunctionality</t>
   </si>
   <si>
+    <t>com.konakart.KonakartParallelTesting.testscripts.ComuterPeripheralsFunctionality</t>
+  </si>
+  <si>
+    <t>com.konakart.KonakartParallelTesting.testscripts.PriceSlideBarFunctionality</t>
+  </si>
+  <si>
+    <t>com.konakart.KonakartParallelTesting.testscripts.TableTest</t>
+  </si>
+  <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>com.konakart.KonakartParallelTesting.testscripts.ComuterPeripheralsFunctionality</t>
-  </si>
-  <si>
-    <t>com.konakart.KonakartParallelTesting.testscripts.PriceSlideBarFunctionality</t>
   </si>
 </sst>
 </file>
@@ -158,9 +161,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20">
@@ -172,6 +175,66 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -179,6 +242,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -186,23 +264,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -217,104 +312,12 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -331,24 +334,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -361,31 +442,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,7 +484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -415,7 +502,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -427,91 +514,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,15 +563,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -580,6 +574,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,148 +630,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1445,13 +1448,13 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="128.857142857143" customWidth="1"/>
   </cols>
@@ -1477,23 +1480,31 @@
         <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5th commit with parallel configuration, multiple url configuration, creating  dynamic xml file by  programatic and also adding listeners for extent report
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -14,13 +14,14 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60">
   <si>
     <t>TestData</t>
   </si>
@@ -134,25 +135,73 @@
     <t>Active</t>
   </si>
   <si>
+    <t>URL</t>
+  </si>
+  <si>
     <t>com.konakart.KonakartParallelTesting.testscripts.HomePageSearchBoxFunctionality</t>
   </si>
   <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>https://www.konakart.com/konakart/Welcome.action</t>
+  </si>
+  <si>
+    <t>com.konakart.KonakartParallelTesting.testscripts.HeroImageFunctionality</t>
+  </si>
+  <si>
+    <t>com.konakart.KonakartParallelTesting.testscripts.ComuterPeripheralsFunctionality</t>
+  </si>
+  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>com.konakart.KonakartParallelTesting.testscripts.HeroImageFunctionality</t>
-  </si>
-  <si>
-    <t>com.konakart.KonakartParallelTesting.testscripts.ComuterPeripheralsFunctionality</t>
-  </si>
-  <si>
     <t>com.konakart.KonakartParallelTesting.testscripts.PriceSlideBarFunctionality</t>
   </si>
   <si>
     <t>com.konakart.KonakartParallelTesting.testscripts.TableTest</t>
   </si>
   <si>
-    <t>N</t>
+    <t>com.konakart.KonakartParallelTesting.testscripts.PhpTravelsTest</t>
+  </si>
+  <si>
+    <t>https://www.phptravels.net/</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>infant</t>
+  </si>
+  <si>
+    <t>Ind</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -161,12 +210,12 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +224,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -191,45 +248,45 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,59 +307,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -318,6 +322,59 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -334,162 +391,180 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -497,24 +572,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -539,15 +596,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -559,6 +607,54 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -582,46 +678,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -630,15 +687,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -648,138 +705,144 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
@@ -1130,22 +1193,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1193,13 +1256,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
@@ -1210,7 +1273,7 @@
       <c r="A2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C2" t="s">
@@ -1338,13 +1401,13 @@
       <c r="D2" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="6" t="s">
         <v>27</v>
       </c>
       <c r="F2" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="6" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1390,10 +1453,10 @@
       <c r="B2" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1415,27 +1478,27 @@
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="4"/>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="7" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="7" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1448,63 +1511,167 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="128.857142857143" customWidth="1"/>
+    <col min="3" max="3" width="54.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="https://www.konakart.com/konakart/Welcome.action"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.konakart.com/konakart/Welcome.action"/>
+    <hyperlink ref="C4" r:id="rId1" display="https://www.konakart.com/konakart/Welcome.action"/>
+    <hyperlink ref="C5" r:id="rId1" display="https://www.konakart.com/konakart/Welcome.action"/>
+    <hyperlink ref="C6" r:id="rId1" display="https://www.konakart.com/konakart/Welcome.action"/>
+    <hyperlink ref="C7" r:id="rId2" display="https://www.phptravels.net/"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="6.14285714285714" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
+        <v>54</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>